<commit_message>
pcb: commit before large routing effort
 - schematic refactor to split preamps to each mic board
 - Mic board and main board are placed
 - no tracks laid
 - critical parts selected
</commit_message>
<xml_diff>
--- a/calc/TestPCBCalcs.xlsx
+++ b/calc/TestPCBCalcs.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Josh\Documents\projects\sound-compass\calc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DC67CE0-B29D-40B8-B999-C70B5705C0CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44E440FB-EF80-4734-87F1-6F039DFEA649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3891D6DE-6321-47E2-B9D1-C2714763336F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{3891D6DE-6321-47E2-B9D1-C2714763336F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Power budget" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
   <si>
     <t>ADC</t>
   </si>
@@ -58,13 +59,28 @@
   </si>
   <si>
     <t>Common mode filter</t>
+  </si>
+  <si>
+    <t>Ohm</t>
+  </si>
+  <si>
+    <t>Input impedance of the THS4531AIRUNR opamp</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>Input DC blocking cap</t>
+  </si>
+  <si>
+    <t>Input differential 1st order HP filter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -74,6 +90,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
@@ -101,10 +125,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -439,30 +464,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F252681F-4686-4D60-B3A0-020294EC3E80}">
-  <dimension ref="A3:C13"/>
+  <dimension ref="A3:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I36" sqref="I36"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -470,7 +495,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -478,7 +503,7 @@
         <v>4.6999999999999997E-8</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -490,7 +515,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -498,7 +523,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>3</v>
       </c>
@@ -506,7 +531,7 @@
         <v>4.7000000000000003E-10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>4</v>
       </c>
@@ -517,6 +542,52 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16">
+        <v>200000</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1">
+        <v>9.9999999999999995E-8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>4</v>
+      </c>
+      <c r="B18">
+        <f>1/(2*PI()*B16*B17)</f>
+        <v>7.9577471545947684</v>
+      </c>
+      <c r="C18" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -527,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1AB8B24-6DA9-4FB1-A27B-395C1B36D7FF}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="I44" sqref="I44"/>
     </sheetView>
   </sheetViews>

</xml_diff>